<commit_message>
Update of the database export for TZ lock
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_tanzania.xlsx
+++ b/inst/extdata/main_dict_tanzania.xlsx
@@ -2670,8 +2670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4959,7 +4959,7 @@
         <v>449</v>
       </c>
       <c r="C79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" s="2">
         <v>1</v>
@@ -5160,7 +5160,7 @@
         <v>562</v>
       </c>
       <c r="C86" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Update for TZ's lock
This version was the one used for the final lock
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_tanzania.xlsx
+++ b/inst/extdata/main_dict_tanzania.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="735">
   <si>
     <t>old</t>
   </si>
@@ -2220,6 +2220,15 @@
   </si>
   <si>
     <t>who_age_ctg</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-e4_1</t>
+  </si>
+  <si>
+    <t>pox_used_cg</t>
+  </si>
+  <si>
+    <t>e4_1</t>
   </si>
 </sst>
 </file>
@@ -2668,10 +2677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O251"/>
+  <dimension ref="A1:O252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
+      <selection activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -8924,10 +8933,10 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" s="25" t="s">
-        <v>616</v>
+        <v>732</v>
       </c>
       <c r="B216" s="25" t="s">
-        <v>128</v>
+        <v>733</v>
       </c>
       <c r="C216" s="2">
         <v>0</v>
@@ -8945,7 +8954,7 @@
         <v>1</v>
       </c>
       <c r="H216" s="25" t="s">
-        <v>284</v>
+        <v>734</v>
       </c>
       <c r="I216" s="3" t="s">
         <v>722</v>
@@ -8953,10 +8962,10 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" s="25" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B217" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C217" s="2">
         <v>0</v>
@@ -8974,7 +8983,7 @@
         <v>1</v>
       </c>
       <c r="H217" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I217" s="3" t="s">
         <v>722</v>
@@ -8982,10 +8991,10 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" s="25" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B218" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C218" s="2">
         <v>0</v>
@@ -9000,10 +9009,10 @@
         <v>1</v>
       </c>
       <c r="G218" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H218" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I218" s="3" t="s">
         <v>722</v>
@@ -9011,10 +9020,10 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" s="25" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B219" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C219" s="2">
         <v>0</v>
@@ -9032,7 +9041,7 @@
         <v>0</v>
       </c>
       <c r="H219" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I219" s="3" t="s">
         <v>722</v>
@@ -9040,10 +9049,10 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" s="25" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B220" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C220" s="2">
         <v>0</v>
@@ -9061,7 +9070,7 @@
         <v>0</v>
       </c>
       <c r="H220" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I220" s="3" t="s">
         <v>722</v>
@@ -9069,10 +9078,10 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" s="25" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B221" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C221" s="2">
         <v>0</v>
@@ -9090,7 +9099,7 @@
         <v>0</v>
       </c>
       <c r="H221" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I221" s="3" t="s">
         <v>722</v>
@@ -9098,10 +9107,10 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" s="25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B222" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C222" s="2">
         <v>0</v>
@@ -9119,7 +9128,7 @@
         <v>0</v>
       </c>
       <c r="H222" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I222" s="3" t="s">
         <v>722</v>
@@ -9127,10 +9136,10 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" s="25" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B223" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C223" s="2">
         <v>0</v>
@@ -9148,7 +9157,7 @@
         <v>0</v>
       </c>
       <c r="H223" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I223" s="3" t="s">
         <v>722</v>
@@ -9156,10 +9165,10 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" s="25" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B224" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C224" s="2">
         <v>0</v>
@@ -9177,7 +9186,7 @@
         <v>0</v>
       </c>
       <c r="H224" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I224" s="3" t="s">
         <v>722</v>
@@ -9185,10 +9194,10 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" s="25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B225" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C225" s="2">
         <v>0</v>
@@ -9206,7 +9215,7 @@
         <v>0</v>
       </c>
       <c r="H225" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I225" s="3" t="s">
         <v>722</v>
@@ -9214,10 +9223,10 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" s="25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B226" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C226" s="2">
         <v>0</v>
@@ -9235,7 +9244,7 @@
         <v>0</v>
       </c>
       <c r="H226" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I226" s="3" t="s">
         <v>722</v>
@@ -9243,10 +9252,10 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" s="25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B227" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C227" s="2">
         <v>0</v>
@@ -9264,7 +9273,7 @@
         <v>0</v>
       </c>
       <c r="H227" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I227" s="3" t="s">
         <v>722</v>
@@ -9272,10 +9281,10 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" s="25" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B228" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C228" s="2">
         <v>0</v>
@@ -9293,7 +9302,7 @@
         <v>0</v>
       </c>
       <c r="H228" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I228" s="3" t="s">
         <v>722</v>
@@ -9301,57 +9310,57 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" s="25" t="s">
+        <v>629</v>
+      </c>
+      <c r="B229" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C229" s="2">
+        <v>0</v>
+      </c>
+      <c r="D229" s="2">
+        <v>0</v>
+      </c>
+      <c r="E229" s="17">
+        <v>1</v>
+      </c>
+      <c r="F229" s="19">
+        <v>1</v>
+      </c>
+      <c r="G229" s="3">
+        <v>0</v>
+      </c>
+      <c r="H229" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="I229" s="3" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A230" s="25" t="s">
         <v>630</v>
       </c>
-      <c r="B229" s="25" t="s">
+      <c r="B230" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="C229" s="2">
-        <v>0</v>
-      </c>
-      <c r="D229" s="2">
-        <v>0</v>
-      </c>
-      <c r="E229" s="17">
-        <v>1</v>
-      </c>
-      <c r="F229" s="19">
-        <v>1</v>
-      </c>
-      <c r="G229" s="3">
-        <v>0</v>
-      </c>
-      <c r="H229" s="25" t="s">
+      <c r="C230" s="2">
+        <v>0</v>
+      </c>
+      <c r="D230" s="2">
+        <v>0</v>
+      </c>
+      <c r="E230" s="17">
+        <v>1</v>
+      </c>
+      <c r="F230" s="19">
+        <v>1</v>
+      </c>
+      <c r="G230" s="3">
+        <v>0</v>
+      </c>
+      <c r="H230" s="25" t="s">
         <v>297</v>
-      </c>
-      <c r="I229" s="3" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A230" s="14" t="s">
-        <v>631</v>
-      </c>
-      <c r="B230" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C230" s="2">
-        <v>0</v>
-      </c>
-      <c r="D230" s="2">
-        <v>0</v>
-      </c>
-      <c r="E230" s="17">
-        <v>1</v>
-      </c>
-      <c r="F230" s="19">
-        <v>1</v>
-      </c>
-      <c r="G230" s="3">
-        <v>0</v>
-      </c>
-      <c r="H230" s="14" t="s">
-        <v>298</v>
       </c>
       <c r="I230" s="3" t="s">
         <v>722</v>
@@ -9359,10 +9368,10 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" s="14" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B231" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C231" s="2">
         <v>0</v>
@@ -9373,14 +9382,14 @@
       <c r="E231" s="17">
         <v>1</v>
       </c>
-      <c r="F231" s="17">
+      <c r="F231" s="19">
         <v>1</v>
       </c>
       <c r="G231" s="3">
         <v>0</v>
       </c>
       <c r="H231" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I231" s="3" t="s">
         <v>722</v>
@@ -9388,10 +9397,10 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" s="14" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B232" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C232" s="2">
         <v>0</v>
@@ -9402,14 +9411,14 @@
       <c r="E232" s="17">
         <v>1</v>
       </c>
-      <c r="F232" s="19">
+      <c r="F232" s="17">
         <v>1</v>
       </c>
       <c r="G232" s="3">
         <v>0</v>
       </c>
       <c r="H232" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I232" s="3" t="s">
         <v>722</v>
@@ -9417,10 +9426,10 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" s="14" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B233" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C233" s="2">
         <v>0</v>
@@ -9438,7 +9447,7 @@
         <v>0</v>
       </c>
       <c r="H233" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I233" s="3" t="s">
         <v>722</v>
@@ -9446,10 +9455,10 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" s="14" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B234" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C234" s="2">
         <v>0</v>
@@ -9467,7 +9476,7 @@
         <v>0</v>
       </c>
       <c r="H234" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I234" s="3" t="s">
         <v>722</v>
@@ -9475,10 +9484,10 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" s="14" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B235" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C235" s="2">
         <v>0</v>
@@ -9496,7 +9505,7 @@
         <v>0</v>
       </c>
       <c r="H235" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I235" s="3" t="s">
         <v>722</v>
@@ -9504,10 +9513,10 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" s="14" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="B236" s="14" t="s">
-        <v>699</v>
+        <v>147</v>
       </c>
       <c r="C236" s="2">
         <v>0</v>
@@ -9525,7 +9534,7 @@
         <v>0</v>
       </c>
       <c r="H236" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I236" s="3" t="s">
         <v>722</v>
@@ -9533,10 +9542,10 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" s="14" t="s">
-        <v>698</v>
+        <v>641</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C237" s="2">
         <v>0</v>
@@ -9562,10 +9571,10 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" s="14" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C238" s="2">
         <v>0</v>
@@ -9591,10 +9600,10 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" s="14" t="s">
-        <v>637</v>
+        <v>700</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>148</v>
+        <v>702</v>
       </c>
       <c r="C239" s="2">
         <v>0</v>
@@ -9612,7 +9621,7 @@
         <v>0</v>
       </c>
       <c r="H239" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I239" s="3" t="s">
         <v>722</v>
@@ -9620,10 +9629,10 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" s="14" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B240" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C240" s="2">
         <v>0</v>
@@ -9641,7 +9650,7 @@
         <v>0</v>
       </c>
       <c r="H240" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I240" s="3" t="s">
         <v>722</v>
@@ -9649,10 +9658,10 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" s="14" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C241" s="2">
         <v>0</v>
@@ -9670,7 +9679,7 @@
         <v>0</v>
       </c>
       <c r="H241" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I241" s="3" t="s">
         <v>722</v>
@@ -9678,57 +9687,57 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242" s="14" t="s">
+        <v>639</v>
+      </c>
+      <c r="B242" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C242" s="2">
+        <v>0</v>
+      </c>
+      <c r="D242" s="2">
+        <v>0</v>
+      </c>
+      <c r="E242" s="17">
+        <v>1</v>
+      </c>
+      <c r="F242" s="19">
+        <v>1</v>
+      </c>
+      <c r="G242" s="3">
+        <v>0</v>
+      </c>
+      <c r="H242" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="I242" s="3" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A243" s="14" t="s">
         <v>640</v>
       </c>
-      <c r="B242" s="14" t="s">
+      <c r="B243" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C242" s="2">
-        <v>0</v>
-      </c>
-      <c r="D242" s="2">
-        <v>0</v>
-      </c>
-      <c r="E242" s="17">
-        <v>1</v>
-      </c>
-      <c r="F242" s="19">
-        <v>1</v>
-      </c>
-      <c r="G242" s="3">
-        <v>0</v>
-      </c>
-      <c r="H242" s="14" t="s">
+      <c r="C243" s="2">
+        <v>0</v>
+      </c>
+      <c r="D243" s="2">
+        <v>0</v>
+      </c>
+      <c r="E243" s="17">
+        <v>1</v>
+      </c>
+      <c r="F243" s="19">
+        <v>1</v>
+      </c>
+      <c r="G243" s="3">
+        <v>0</v>
+      </c>
+      <c r="H243" s="14" t="s">
         <v>308</v>
-      </c>
-      <c r="I242" s="3" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A243" s="15" t="s">
-        <v>642</v>
-      </c>
-      <c r="B243" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C243" s="2">
-        <v>0</v>
-      </c>
-      <c r="D243" s="2">
-        <v>0</v>
-      </c>
-      <c r="E243" s="17">
-        <v>1</v>
-      </c>
-      <c r="F243" s="19">
-        <v>1</v>
-      </c>
-      <c r="G243" s="3">
-        <v>0</v>
-      </c>
-      <c r="H243" s="15" t="s">
-        <v>309</v>
       </c>
       <c r="I243" s="3" t="s">
         <v>722</v>
@@ -9736,10 +9745,10 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244" s="15" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B244" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C244" s="2">
         <v>0</v>
@@ -9757,7 +9766,7 @@
         <v>0</v>
       </c>
       <c r="H244" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I244" s="3" t="s">
         <v>722</v>
@@ -9765,10 +9774,10 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B245" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C245" s="2">
         <v>0</v>
@@ -9786,7 +9795,7 @@
         <v>0</v>
       </c>
       <c r="H245" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I245" s="3" t="s">
         <v>722</v>
@@ -9794,10 +9803,10 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246" s="15" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B246" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C246" s="2">
         <v>0</v>
@@ -9815,7 +9824,7 @@
         <v>0</v>
       </c>
       <c r="H246" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I246" s="3" t="s">
         <v>722</v>
@@ -9823,10 +9832,10 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247" s="15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B247" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C247" s="2">
         <v>0</v>
@@ -9844,7 +9853,7 @@
         <v>0</v>
       </c>
       <c r="H247" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I247" s="3" t="s">
         <v>722</v>
@@ -9852,10 +9861,10 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248" s="15" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B248" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C248" s="2">
         <v>0</v>
@@ -9873,7 +9882,7 @@
         <v>0</v>
       </c>
       <c r="H248" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I248" s="3" t="s">
         <v>722</v>
@@ -9881,10 +9890,10 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249" s="15" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B249" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C249" s="2">
         <v>0</v>
@@ -9902,7 +9911,7 @@
         <v>0</v>
       </c>
       <c r="H249" s="15" t="s">
-        <v>203</v>
+        <v>314</v>
       </c>
       <c r="I249" s="3" t="s">
         <v>722</v>
@@ -9910,59 +9919,88 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="B250" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C250" s="2">
+        <v>0</v>
+      </c>
+      <c r="D250" s="2">
+        <v>0</v>
+      </c>
+      <c r="E250" s="17">
+        <v>1</v>
+      </c>
+      <c r="F250" s="19">
+        <v>1</v>
+      </c>
+      <c r="G250" s="3">
+        <v>0</v>
+      </c>
+      <c r="H250" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="I250" s="3" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A251" s="15" t="s">
         <v>649</v>
       </c>
-      <c r="B250" s="15" t="s">
+      <c r="B251" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C250" s="2">
-        <v>0</v>
-      </c>
-      <c r="D250" s="2">
-        <v>0</v>
-      </c>
-      <c r="E250" s="17">
-        <v>1</v>
-      </c>
-      <c r="F250" s="17">
-        <v>1</v>
-      </c>
-      <c r="G250" s="3">
-        <v>0</v>
-      </c>
-      <c r="H250" s="15" t="s">
+      <c r="C251" s="2">
+        <v>0</v>
+      </c>
+      <c r="D251" s="2">
+        <v>0</v>
+      </c>
+      <c r="E251" s="17">
+        <v>1</v>
+      </c>
+      <c r="F251" s="17">
+        <v>1</v>
+      </c>
+      <c r="G251" s="3">
+        <v>0</v>
+      </c>
+      <c r="H251" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="I250" s="3" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A251" s="5" t="s">
+      <c r="I251" s="3" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A252" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="B251" s="5" t="s">
+      <c r="B252" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="C251" s="2">
-        <v>1</v>
-      </c>
-      <c r="D251" s="2">
-        <v>1</v>
-      </c>
-      <c r="E251" s="4">
-        <v>1</v>
-      </c>
-      <c r="F251" s="3">
-        <v>1</v>
-      </c>
-      <c r="G251" s="3">
-        <v>0</v>
-      </c>
-      <c r="H251" s="5" t="s">
+      <c r="C252" s="2">
+        <v>1</v>
+      </c>
+      <c r="D252" s="2">
+        <v>1</v>
+      </c>
+      <c r="E252" s="4">
+        <v>1</v>
+      </c>
+      <c r="F252" s="3">
+        <v>1</v>
+      </c>
+      <c r="G252" s="3">
+        <v>0</v>
+      </c>
+      <c r="H252" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="I251" s="3" t="s">
+      <c r="I252" s="3" t="s">
         <v>723</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update dictionaries for more consistency
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_tanzania.xlsx
+++ b/inst/extdata/main_dict_tanzania.xlsx
@@ -2407,7 +2407,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2685,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155:XFD155"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M240" sqref="M240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10037,6 +10048,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:G253">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update dictionary for cross-country consistency
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_tanzania.xlsx
+++ b/inst/extdata/main_dict_tanzania.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10890"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2192,24 +2192,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>col_integer()</t>
-  </si>
-  <si>
-    <t>col_character()</t>
-  </si>
-  <si>
-    <t>col_date()</t>
-  </si>
-  <si>
-    <t>col_datetime()</t>
-  </si>
-  <si>
-    <t>col_time()</t>
-  </si>
-  <si>
-    <t>col_double()</t>
-  </si>
-  <si>
     <t>crfs-t02b-contact_start</t>
   </si>
   <si>
@@ -2235,6 +2217,24 @@
   </si>
   <si>
     <t>form_version</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>nominal</t>
   </si>
 </sst>
 </file>
@@ -2696,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O253"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M240" sqref="M240"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2769,7 +2769,7 @@
         <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>724</v>
+        <v>7</v>
       </c>
       <c r="O2" s="29"/>
     </row>
@@ -2799,7 +2799,7 @@
         <v>27</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -2828,7 +2828,7 @@
         <v>25</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2857,7 +2857,7 @@
         <v>429</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -2886,7 +2886,7 @@
         <v>613</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2915,7 +2915,7 @@
         <v>550</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2944,15 +2944,15 @@
         <v>495</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -2970,10 +2970,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -3002,7 +3002,7 @@
         <v>495</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>726</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -3031,7 +3031,7 @@
         <v>536</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -3060,7 +3060,7 @@
         <v>536</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>726</v>
+        <v>734</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -3089,7 +3089,7 @@
         <v>537</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -3118,7 +3118,7 @@
         <v>539</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3147,7 +3147,7 @@
         <v>541</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -3176,7 +3176,7 @@
         <v>543</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -3205,7 +3205,7 @@
         <v>546</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -3234,7 +3234,7 @@
         <v>651</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -3263,7 +3263,7 @@
         <v>653</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -3292,7 +3292,7 @@
         <v>315</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -3321,7 +3321,7 @@
         <v>163</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -3350,7 +3350,7 @@
         <v>164</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>724</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -3379,7 +3379,7 @@
         <v>430</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>724</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -3408,7 +3408,7 @@
         <v>165</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>724</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -3437,7 +3437,7 @@
         <v>36</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>724</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -3466,7 +3466,7 @@
         <v>439</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -3495,7 +3495,7 @@
         <v>166</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -3524,7 +3524,7 @@
         <v>167</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -3553,7 +3553,7 @@
         <v>168</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -3582,7 +3582,7 @@
         <v>436</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -3611,7 +3611,7 @@
         <v>170</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -3640,7 +3640,7 @@
         <v>171</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -3669,7 +3669,7 @@
         <v>172</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -3677,7 +3677,7 @@
         <v>323</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -3698,7 +3698,7 @@
         <v>169</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -3727,7 +3727,7 @@
         <v>173</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -3756,7 +3756,7 @@
         <v>174</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -3785,7 +3785,7 @@
         <v>8</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -3814,7 +3814,7 @@
         <v>175</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -3843,7 +3843,7 @@
         <v>176</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -3872,7 +3872,7 @@
         <v>177</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -3901,7 +3901,7 @@
         <v>178</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -3930,7 +3930,7 @@
         <v>454</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -3959,7 +3959,7 @@
         <v>179</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -3988,7 +3988,7 @@
         <v>180</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -4017,7 +4017,7 @@
         <v>181</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -4046,7 +4046,7 @@
         <v>182</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -4075,7 +4075,7 @@
         <v>455</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -4104,7 +4104,7 @@
         <v>184</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -4133,7 +4133,7 @@
         <v>185</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -4162,7 +4162,7 @@
         <v>186</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -4191,7 +4191,7 @@
         <v>187</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -4220,7 +4220,7 @@
         <v>188</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -4249,7 +4249,7 @@
         <v>189</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -4278,7 +4278,7 @@
         <v>190</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -4307,7 +4307,7 @@
         <v>191</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -4336,7 +4336,7 @@
         <v>192</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -4365,7 +4365,7 @@
         <v>193</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -4394,7 +4394,7 @@
         <v>194</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -4423,7 +4423,7 @@
         <v>558</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -4452,7 +4452,7 @@
         <v>559</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -4481,7 +4481,7 @@
         <v>195</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -4510,7 +4510,7 @@
         <v>720</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -4539,7 +4539,7 @@
         <v>196</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -4568,7 +4568,7 @@
         <v>197</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -4597,7 +4597,7 @@
         <v>198</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -4626,7 +4626,7 @@
         <v>661</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -4655,7 +4655,7 @@
         <v>506</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -4684,7 +4684,7 @@
         <v>656</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -4713,7 +4713,7 @@
         <v>199</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -4742,7 +4742,7 @@
         <v>200</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -4771,7 +4771,7 @@
         <v>433</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -4800,7 +4800,7 @@
         <v>434</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -4829,7 +4829,7 @@
         <v>444</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -4858,7 +4858,7 @@
         <v>201</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -4887,7 +4887,7 @@
         <v>567</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -4916,7 +4916,7 @@
         <v>204</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -4945,7 +4945,7 @@
         <v>205</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -4974,7 +4974,7 @@
         <v>206</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -5003,7 +5003,7 @@
         <v>449</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -5032,7 +5032,7 @@
         <v>451</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -5059,7 +5059,7 @@
       </c>
       <c r="H81" s="11"/>
       <c r="I81" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -5088,7 +5088,7 @@
         <v>446</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
@@ -5117,7 +5117,7 @@
         <v>498</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -5146,7 +5146,7 @@
         <v>503</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -5175,7 +5175,7 @@
         <v>504</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -5204,7 +5204,7 @@
         <v>562</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -5233,7 +5233,7 @@
         <v>565</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -5262,7 +5262,7 @@
         <v>718</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -5291,7 +5291,7 @@
         <v>207</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -5320,7 +5320,7 @@
         <v>208</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
@@ -5349,7 +5349,7 @@
         <v>209</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -5378,7 +5378,7 @@
         <v>210</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -5407,7 +5407,7 @@
         <v>211</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
@@ -5436,7 +5436,7 @@
         <v>212</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -5465,7 +5465,7 @@
         <v>213</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
@@ -5494,7 +5494,7 @@
         <v>214</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -5523,7 +5523,7 @@
         <v>227</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -5552,7 +5552,7 @@
         <v>228</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -5581,7 +5581,7 @@
         <v>229</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -5610,7 +5610,7 @@
         <v>230</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -5639,7 +5639,7 @@
         <v>231</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
@@ -5668,7 +5668,7 @@
         <v>232</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -5697,7 +5697,7 @@
         <v>233</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -5726,7 +5726,7 @@
         <v>234</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
@@ -5755,7 +5755,7 @@
         <v>235</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
@@ -5784,7 +5784,7 @@
         <v>236</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
@@ -5813,7 +5813,7 @@
         <v>237</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
@@ -5842,7 +5842,7 @@
         <v>238</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
@@ -5871,7 +5871,7 @@
         <v>239</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
@@ -5900,7 +5900,7 @@
         <v>240</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -5929,7 +5929,7 @@
         <v>241</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
@@ -5958,7 +5958,7 @@
         <v>242</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
@@ -5987,7 +5987,7 @@
         <v>243</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
@@ -6016,7 +6016,7 @@
         <v>244</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
@@ -6045,7 +6045,7 @@
         <v>245</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -6074,7 +6074,7 @@
         <v>246</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -6103,7 +6103,7 @@
         <v>247</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
@@ -6132,7 +6132,7 @@
         <v>276</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -6161,7 +6161,7 @@
         <v>574</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
@@ -6190,7 +6190,7 @@
         <v>569</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
@@ -6219,7 +6219,7 @@
         <v>215</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
@@ -6248,7 +6248,7 @@
         <v>216</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
@@ -6277,7 +6277,7 @@
         <v>217</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
@@ -6306,7 +6306,7 @@
         <v>218</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
@@ -6335,7 +6335,7 @@
         <v>219</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
@@ -6364,7 +6364,7 @@
         <v>220</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -6393,7 +6393,7 @@
         <v>221</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
@@ -6422,7 +6422,7 @@
         <v>222</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
@@ -6451,7 +6451,7 @@
         <v>223</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
@@ -6480,7 +6480,7 @@
         <v>224</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
@@ -6509,7 +6509,7 @@
         <v>225</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
@@ -6538,7 +6538,7 @@
         <v>226</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
@@ -6567,7 +6567,7 @@
         <v>248</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
@@ -6596,7 +6596,7 @@
         <v>249</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
@@ -6625,7 +6625,7 @@
         <v>250</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
@@ -6654,7 +6654,7 @@
         <v>251</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
@@ -6683,7 +6683,7 @@
         <v>252</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
@@ -6712,7 +6712,7 @@
         <v>253</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
@@ -6741,7 +6741,7 @@
         <v>254</v>
       </c>
       <c r="I139" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
@@ -6770,7 +6770,7 @@
         <v>255</v>
       </c>
       <c r="I140" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
@@ -6799,7 +6799,7 @@
         <v>256</v>
       </c>
       <c r="I141" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
@@ -6828,7 +6828,7 @@
         <v>257</v>
       </c>
       <c r="I142" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
@@ -6857,7 +6857,7 @@
         <v>258</v>
       </c>
       <c r="I143" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
@@ -6886,7 +6886,7 @@
         <v>259</v>
       </c>
       <c r="I144" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
@@ -6915,7 +6915,7 @@
         <v>260</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
@@ -6944,7 +6944,7 @@
         <v>261</v>
       </c>
       <c r="I146" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
@@ -6973,7 +6973,7 @@
         <v>262</v>
       </c>
       <c r="I147" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
@@ -7002,7 +7002,7 @@
         <v>263</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
@@ -7031,7 +7031,7 @@
         <v>264</v>
       </c>
       <c r="I149" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
@@ -7060,7 +7060,7 @@
         <v>265</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
@@ -7089,7 +7089,7 @@
         <v>266</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
@@ -7118,7 +7118,7 @@
         <v>267</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
@@ -7147,7 +7147,7 @@
         <v>268</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
@@ -7176,7 +7176,7 @@
         <v>269</v>
       </c>
       <c r="I154" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
@@ -7205,7 +7205,7 @@
         <v>663</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
@@ -7234,7 +7234,7 @@
         <v>114</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
@@ -7263,7 +7263,7 @@
         <v>279</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
@@ -7292,7 +7292,7 @@
         <v>697</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
@@ -7321,7 +7321,7 @@
         <v>509</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
@@ -7350,7 +7350,7 @@
         <v>511</v>
       </c>
       <c r="I160" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
@@ -7379,7 +7379,7 @@
         <v>270</v>
       </c>
       <c r="I161" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
@@ -7408,7 +7408,7 @@
         <v>280</v>
       </c>
       <c r="I162" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
@@ -7437,7 +7437,7 @@
         <v>281</v>
       </c>
       <c r="I163" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
@@ -7466,7 +7466,7 @@
         <v>533</v>
       </c>
       <c r="I164" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
@@ -7495,7 +7495,7 @@
         <v>271</v>
       </c>
       <c r="I165" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
@@ -7524,7 +7524,7 @@
         <v>272</v>
       </c>
       <c r="I166" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
@@ -7553,7 +7553,7 @@
         <v>532</v>
       </c>
       <c r="I167" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
@@ -7582,7 +7582,7 @@
         <v>273</v>
       </c>
       <c r="I168" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
@@ -7611,7 +7611,7 @@
         <v>665</v>
       </c>
       <c r="I169" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
@@ -7640,7 +7640,7 @@
         <v>577</v>
       </c>
       <c r="I170" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
@@ -7669,7 +7669,7 @@
         <v>580</v>
       </c>
       <c r="I171" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
@@ -7698,7 +7698,7 @@
         <v>583</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
@@ -7727,7 +7727,7 @@
         <v>586</v>
       </c>
       <c r="I173" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
@@ -7756,7 +7756,7 @@
         <v>589</v>
       </c>
       <c r="I174" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
@@ -7785,7 +7785,7 @@
         <v>592</v>
       </c>
       <c r="I175" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
@@ -7814,7 +7814,7 @@
         <v>673</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
@@ -7843,7 +7843,7 @@
         <v>595</v>
       </c>
       <c r="I177" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
@@ -7872,7 +7872,7 @@
         <v>598</v>
       </c>
       <c r="I178" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
@@ -7901,7 +7901,7 @@
         <v>601</v>
       </c>
       <c r="I179" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
@@ -7930,7 +7930,7 @@
         <v>668</v>
       </c>
       <c r="I180" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
@@ -7959,7 +7959,7 @@
         <v>604</v>
       </c>
       <c r="I181" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
@@ -7988,7 +7988,7 @@
         <v>606</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
@@ -8017,7 +8017,7 @@
         <v>609</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
@@ -8046,7 +8046,7 @@
         <v>612</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
@@ -8075,7 +8075,7 @@
         <v>676</v>
       </c>
       <c r="I185" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
@@ -8104,7 +8104,7 @@
         <v>679</v>
       </c>
       <c r="I186" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
@@ -8133,7 +8133,7 @@
         <v>684</v>
       </c>
       <c r="I187" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
@@ -8162,7 +8162,7 @@
         <v>685</v>
       </c>
       <c r="I188" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
@@ -8191,7 +8191,7 @@
         <v>688</v>
       </c>
       <c r="I189" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
@@ -8220,7 +8220,7 @@
         <v>690</v>
       </c>
       <c r="I190" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
@@ -8249,7 +8249,7 @@
         <v>694</v>
       </c>
       <c r="I191" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
@@ -8278,7 +8278,7 @@
         <v>274</v>
       </c>
       <c r="I192" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
@@ -8307,7 +8307,7 @@
         <v>275</v>
       </c>
       <c r="I193" s="3" t="s">
-        <v>722</v>
+        <v>732</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
@@ -8336,7 +8336,7 @@
         <v>459</v>
       </c>
       <c r="I194" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.3">
@@ -8365,7 +8365,7 @@
         <v>460</v>
       </c>
       <c r="I195" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.3">
@@ -8394,7 +8394,7 @@
         <v>461</v>
       </c>
       <c r="I196" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
@@ -8423,7 +8423,7 @@
         <v>462</v>
       </c>
       <c r="I197" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
@@ -8452,7 +8452,7 @@
         <v>463</v>
       </c>
       <c r="I198" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
@@ -8481,7 +8481,7 @@
         <v>464</v>
       </c>
       <c r="I199" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
@@ -8510,7 +8510,7 @@
         <v>465</v>
       </c>
       <c r="I200" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
@@ -8539,7 +8539,7 @@
         <v>466</v>
       </c>
       <c r="I201" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
@@ -8568,7 +8568,7 @@
         <v>467</v>
       </c>
       <c r="I202" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
@@ -8597,7 +8597,7 @@
         <v>468</v>
       </c>
       <c r="I203" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.3">
@@ -8626,7 +8626,7 @@
         <v>469</v>
       </c>
       <c r="I204" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.3">
@@ -8655,7 +8655,7 @@
         <v>470</v>
       </c>
       <c r="I205" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.3">
@@ -8684,7 +8684,7 @@
         <v>471</v>
       </c>
       <c r="I206" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.3">
@@ -8713,7 +8713,7 @@
         <v>472</v>
       </c>
       <c r="I207" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.3">
@@ -8742,7 +8742,7 @@
         <v>473</v>
       </c>
       <c r="I208" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
@@ -8771,7 +8771,7 @@
         <v>474</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
@@ -8800,7 +8800,7 @@
         <v>475</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
@@ -8829,7 +8829,7 @@
         <v>476</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
@@ -8858,7 +8858,7 @@
         <v>277</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
@@ -8887,7 +8887,7 @@
         <v>278</v>
       </c>
       <c r="I213" s="3" t="s">
-        <v>722</v>
+        <v>732</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
@@ -8916,7 +8916,7 @@
         <v>282</v>
       </c>
       <c r="I214" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
@@ -8945,15 +8945,15 @@
         <v>283</v>
       </c>
       <c r="I215" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" s="25" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="B216" s="25" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="C216" s="2">
         <v>0</v>
@@ -8971,10 +8971,10 @@
         <v>1</v>
       </c>
       <c r="H216" s="25" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
@@ -9003,7 +9003,7 @@
         <v>284</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
@@ -9032,7 +9032,7 @@
         <v>285</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
@@ -9061,7 +9061,7 @@
         <v>286</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
@@ -9090,7 +9090,7 @@
         <v>287</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
@@ -9119,7 +9119,7 @@
         <v>288</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
@@ -9148,7 +9148,7 @@
         <v>289</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
@@ -9177,7 +9177,7 @@
         <v>290</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
@@ -9206,7 +9206,7 @@
         <v>291</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
@@ -9235,7 +9235,7 @@
         <v>292</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
@@ -9264,7 +9264,7 @@
         <v>293</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
@@ -9293,7 +9293,7 @@
         <v>294</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
@@ -9322,7 +9322,7 @@
         <v>295</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
@@ -9351,7 +9351,7 @@
         <v>296</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
@@ -9380,7 +9380,7 @@
         <v>297</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
@@ -9409,7 +9409,7 @@
         <v>298</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
@@ -9438,7 +9438,7 @@
         <v>299</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
@@ -9467,7 +9467,7 @@
         <v>300</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
@@ -9496,7 +9496,7 @@
         <v>301</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
@@ -9525,7 +9525,7 @@
         <v>302</v>
       </c>
       <c r="I235" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
@@ -9554,7 +9554,7 @@
         <v>303</v>
       </c>
       <c r="I236" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
@@ -9583,7 +9583,7 @@
         <v>304</v>
       </c>
       <c r="I237" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
@@ -9612,7 +9612,7 @@
         <v>304</v>
       </c>
       <c r="I238" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
@@ -9641,7 +9641,7 @@
         <v>304</v>
       </c>
       <c r="I239" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
@@ -9670,7 +9670,7 @@
         <v>305</v>
       </c>
       <c r="I240" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.3">
@@ -9699,7 +9699,7 @@
         <v>306</v>
       </c>
       <c r="I241" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.3">
@@ -9728,7 +9728,7 @@
         <v>307</v>
       </c>
       <c r="I242" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.3">
@@ -9757,7 +9757,7 @@
         <v>308</v>
       </c>
       <c r="I243" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.3">
@@ -9786,7 +9786,7 @@
         <v>309</v>
       </c>
       <c r="I244" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.3">
@@ -9815,7 +9815,7 @@
         <v>310</v>
       </c>
       <c r="I245" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">
@@ -9844,7 +9844,7 @@
         <v>311</v>
       </c>
       <c r="I246" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.3">
@@ -9873,7 +9873,7 @@
         <v>312</v>
       </c>
       <c r="I247" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
@@ -9902,7 +9902,7 @@
         <v>313</v>
       </c>
       <c r="I248" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.3">
@@ -9931,7 +9931,7 @@
         <v>314</v>
       </c>
       <c r="I249" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.3">
@@ -9960,7 +9960,7 @@
         <v>203</v>
       </c>
       <c r="I250" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.3">
@@ -9989,7 +9989,7 @@
         <v>202</v>
       </c>
       <c r="I251" s="3" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.3">
@@ -10018,15 +10018,15 @@
         <v>554</v>
       </c>
       <c r="I252" s="3" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A253" s="5" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="C253" s="2">
         <v>1</v>
@@ -10044,7 +10044,7 @@
         <v>1</v>
       </c>
       <c r="H253" s="5" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>